<commit_message>
Update Weighted Evaluation Table for Project Selection.xlsx
Added more weighting objectives to the table.
</commit_message>
<xml_diff>
--- a/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
+++ b/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C345941-9DDE-4E0A-921D-7630BC4CBBA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD12BDC3-E537-44AC-A841-24F9BB7EA84E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="20">
   <si>
     <t>Smart Connected Cat Feeding &amp; Monitoring System</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>Mobile Application</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Image Processing</t>
+  </si>
+  <si>
+    <t>Inexpensive</t>
+  </si>
+  <si>
+    <t>Multidisciplinary</t>
   </si>
 </sst>
 </file>
@@ -400,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,259 +506,419 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>3</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19">
-        <f>(B3+H3+B11+H11+B19)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f>(C3+I3+C11+I11+C19)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f>(D3+J3+D11+J11+D19)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <f>(E3+K3+E11+K11+E19)/50</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20">
-        <f>(B4+H4+B12+H12+B20)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" ref="I20:K20" si="0">(C4+I4+C12+I12+C20)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <f>(B5+H5+B13+H13+B21)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f t="shared" ref="I21:K21" si="1">(C5+I5+C13+I13+C21)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22">
-        <f>(B6+H6+B14+H14+B22)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f t="shared" ref="I22:K22" si="2">(C6+I6+C14+I14+C22)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <f>(B3+H3+B14+H14+B25)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>(C3+I3+C14+I14+C25)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>(D3+J3+D14+J14+D25)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>(E3+K3+E14+K14+E25)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <f>(B4+H4+B15+H15+B26)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>(C4+I4+C15+I15+C26)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>(D4+J4+D15+J15+D26)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>(E4+K4+E15+K15+E26)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <f>(B5+H5+B16+H16+B27)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>(C5+I5+C16+I16+C27)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>(D5+J5+D16+J16+D27)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>(E5+K5+E16+K16+E27)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <f>(B6+H6+B17+H17+B28)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>(C6+I6+C17+I17+C28)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>(D6+J6+D17+J17+D28)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>(E6+K6+E17+K17+E28)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>8</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G29" t="s">
         <v>8</v>
       </c>
-      <c r="H23">
-        <f>(B7+H7+B15+H15+B23)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f t="shared" ref="I23:K23" si="3">(C7+I7+C15+I15+C23)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="H29">
+        <f>(B7+H7+B18+H18+B29)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f>(C7+I7+C18+I18+C29)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f>(D7+J7+D18+J18+D29)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>(E7+K7+E18+K18+E29)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>15</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G30" t="s">
         <v>15</v>
       </c>
-      <c r="H24">
-        <f>(B8+H8+B16+H16+B24)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f t="shared" ref="I24:K24" si="4">(C8+I8+C16+I16+C24)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="4"/>
+      <c r="H30">
+        <f>(B8+H8+B19+H19+B30)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f>(C8+I8+C19+I19+C30)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f>(D8+J8+D19+J19+D30)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>(E8+K8+E19+K19+E30)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31">
+        <f>(B9 + H9 + B20 + H20  + B31)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f>(C9 + I9 + C20 + I20 +  C31)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f>(D9 + J9 + D20 + J20 + D31)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f>(E9 + K9 + E20 + K20 + E31)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32">
+        <f>(B10 + H10 + B21 + H21 + B32)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f>(C10 + I10 + C21 + I21 + C32)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f>(D10 + J10 + D21 + J21 + D32)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f>(E10 + K10 + E21 + K21 + E32)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33">
+        <f>(B11 + H11 + B22 + H22 + B33)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f>(C11 + I11 + C22 + I22 + C33)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f>(D11 + J11 + D22 + J22 + D33)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f>(E11 + K11 + E22 + K22 + E33)/50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34">
+        <f>(B12 + H12 + B23 + H23 + B34)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f>(C12 + I12 + C23 + I23 + C34)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f>(D12 + J12 + D23 + J23 + D34)/50</f>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>(E12 + K12 + E23 + K23 + E34)/50</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Weighted Evaluation Table for Project Selection
Please pull origin, gice scores for your section between 1-10. 0 is not available.
Then Push the document to the master branch.
</commit_message>
<xml_diff>
--- a/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
+++ b/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDEA151-0F1C-44D3-9E19-0BE2E6F04D2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC0D4CB-6FAD-4508-8FB2-9C2C79065F5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
   <si>
     <t>Smart Connected Cat Feeding &amp; Monitoring System</t>
   </si>
@@ -40,21 +40,6 @@
     <t>Where am I</t>
   </si>
   <si>
-    <t>Mechanic Design</t>
-  </si>
-  <si>
-    <t>Software Design</t>
-  </si>
-  <si>
-    <t>Sensors&amp;Electronic Design</t>
-  </si>
-  <si>
-    <t>Motors&amp;Motor Drivers</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
     <t>Elif Merve ÖZALP</t>
   </si>
   <si>
@@ -73,22 +58,28 @@
     <t>Overall</t>
   </si>
   <si>
-    <t>Mobile Application</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>Image Processing</t>
-  </si>
-  <si>
-    <t>Inexpensive</t>
-  </si>
-  <si>
     <t>Multidisciplinary</t>
   </si>
   <si>
-    <t>Fun</t>
+    <t>Software Based</t>
+  </si>
+  <si>
+    <t>Hardware Based</t>
+  </si>
+  <si>
+    <t>Adoptability to Everyday Life</t>
+  </si>
+  <si>
+    <t>Mechanic Based</t>
+  </si>
+  <si>
+    <t>Open to Improvement</t>
+  </si>
+  <si>
+    <t>Enjoyable</t>
+  </si>
+  <si>
+    <t>Marketable</t>
   </si>
 </sst>
 </file>
@@ -415,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K37"/>
+  <dimension ref="A2:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
@@ -431,7 +422,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -446,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
@@ -463,42 +454,42 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -525,427 +516,323 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
+    <row r="12" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>3</v>
+      <c r="G14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="G22" t="s">
-        <v>17</v>
+    </row>
+    <row r="22" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <f>(B3+H3+B13+H13+B23)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:K30" si="0">(C3+I3+C13+I13+C23)/50</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H30" si="1">(B4+H4+B14+H14+B24)/50</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="144.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>3</v>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H27">
-        <f>(B3+H3+B15+H15+B27)/50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I27">
-        <f>(C3+I3+C15+I15+C27)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J27">
-        <f>(D3+J3+D15+J15+D27)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K27">
-        <f>(E3+K3+E15+K15+E27)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H28">
-        <f>(B4+H4+B16+H16+B28)/50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I28">
-        <f>(C4+I4+C16+I16+C28)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J28">
-        <f>(D4+J4+D16+J16+D28)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K28">
-        <f>(E4+K4+E16+K16+E28)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H29">
-        <f>(B5+H5+B17+H17+B29)/50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I29">
-        <f>(C5+I5+C17+I17+C29)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J29">
-        <f>(D5+J5+D17+J17+D29)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K29">
-        <f>(E5+K5+E17+K17+E29)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H30">
-        <f>(B6+H6+B18+H18+B30)/50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I30">
-        <f>(C6+I6+C18+I18+C30)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J30">
-        <f>(D6+J6+D18+J18+D30)/50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K30">
-        <f>(E6+K6+E18+K18+E30)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31">
-        <f>(B7+H7+B19+H19+B31)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <f>(C7+I7+C19+I19+C31)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <f>(D7+J7+D19+J19+D31)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <f>(E7+K7+E19+K19+E31)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32">
-        <f>(B8+H8+B20+H20+B32)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <f>(C8+I8+C20+I20+C32)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <f>(D8+J8+D20+J20+D32)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <f>(E8+K8+E20+K20+E32)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33">
-        <f>(B9 + H9 + B21 + H21  + B33)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <f>(C9 + I9 + C21 + I21 +  C33)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <f>(D9 + J9 + D21 + J21 + D33)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <f>(E9 + K9 + E21 + K21 + E33)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34">
-        <f>(B10 + H10 + B22 + H22 + B34)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <f>(C10 + I10 + C22 + I22 + C34)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <f>(D10 + J10 + D22 + J22 + D34)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <f>(E10 + K10 + E22 + K22 + E34)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35">
-        <f>(B11 + H11 + B23 + H23 + B35)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <f>(C11 + I11 + C23 + I23 + C35)/50</f>
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <f>(D11 + J11 + D23 + J23 + D35)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <f>(E11 + K11 + E23 + K23 + E35)/50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37">
-        <f t="shared" ref="H37:I37" si="0">(B13 + H13 + B25 + H25 + B37)/50</f>
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <f t="shared" ref="J37:K37" si="1">(D13 + J13 + D25 + J25 + D37)/50</f>
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Filled the weighted table
</commit_message>
<xml_diff>
--- a/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
+++ b/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36435D29-CEF3-4DE4-87F4-8FB7575F0EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560ABEC6-9416-4009-93FC-A0D95203D86F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,17 +497,26 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J3">
         <f>(I3/I11)</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K3" t="s">
         <v>11</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -518,12 +527,27 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
       <c r="J4">
         <f>(I4/I11)</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -534,12 +558,27 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
       <c r="J5">
         <f>(I5/I11)</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -550,12 +589,27 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
       <c r="J6">
         <f>(I6/I11)</f>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -566,12 +620,27 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
       <c r="J7">
         <f>(I7/I11)</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -582,12 +651,27 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
       <c r="J8">
         <f>(I8/I11)</f>
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="K8" t="s">
         <v>15</v>
+      </c>
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -598,12 +682,27 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
       <c r="J9">
         <f>(I9/I11)</f>
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="K9" t="s">
         <v>16</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -614,12 +713,27 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
       <c r="J10">
         <f>(I10/I11)</f>
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="K10" t="s">
         <v>17</v>
+      </c>
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -629,7 +743,7 @@
       </c>
       <c r="I11">
         <f>(I3+I4+I5+I6+I7+I8+I9+I10)</f>
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="144.75" x14ac:dyDescent="0.25">
@@ -705,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="L13">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -999,26 +1113,26 @@
       </c>
       <c r="I23">
         <f>(B3+J3+B13+J13+B23)/5</f>
-        <v>0.62690909090909097</v>
+        <v>0.44690909090909087</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
       </c>
       <c r="L23">
         <f>((D3+L3+D13+L13+D23)/5)*I23</f>
-        <v>6.018327272727273</v>
+        <v>3.3071272727272727</v>
       </c>
       <c r="M23">
         <f>((E3+M3+E13+M13+E23)/5)*I23</f>
-        <v>1.3792000000000002</v>
+        <v>1.6088727272727272</v>
       </c>
       <c r="N23">
         <f>((F3+N3+F13+N13+F23)/5)*I23</f>
-        <v>1.880727272727273</v>
+        <v>1.9663999999999999</v>
       </c>
       <c r="O23">
         <f>((G3+O3+G13+O13+G23)/5)*I23</f>
-        <v>2.0061090909090913</v>
+        <v>2.2345454545454544</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1046,26 +1160,26 @@
       </c>
       <c r="I24">
         <f t="shared" ref="I24:I30" si="0">(B4+J4+B14+J14+B24)/5</f>
-        <v>4.2181818181818181E-2</v>
+        <v>6.2181818181818185E-2</v>
       </c>
       <c r="K24" t="s">
         <v>12</v>
       </c>
       <c r="L24">
         <f t="shared" ref="L24:L30" si="1">((D4+L4+D14+L14+D24)/5)*I24</f>
-        <v>3.3745454545454544E-2</v>
+        <v>9.9490909090909102E-2</v>
       </c>
       <c r="M24">
         <f t="shared" ref="M24:M30" si="2">((E4+M4+E14+M14+E24)/5)*I24</f>
-        <v>7.5927272727272732E-2</v>
+        <v>0.21141818181818184</v>
       </c>
       <c r="N24">
         <f t="shared" ref="N24:N30" si="3">((F4+N4+F14+N14+F24)/5)*I24</f>
-        <v>0.10123636363636364</v>
+        <v>0.24872727272727274</v>
       </c>
       <c r="O24">
         <f t="shared" ref="O24:O30" si="4">((G4+O4+G14+O14+G24)/5)*I24</f>
-        <v>0.1181090909090909</v>
+        <v>0.27360000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1093,26 +1207,26 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>5.3454545454545456E-2</v>
+        <v>7.3454545454545467E-2</v>
       </c>
       <c r="K25" t="s">
         <v>10</v>
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>8.552727272727273E-2</v>
+        <v>0.14690909090909093</v>
       </c>
       <c r="M25">
         <f t="shared" si="2"/>
-        <v>0.17105454545454546</v>
+        <v>0.36727272727272731</v>
       </c>
       <c r="N25">
         <f t="shared" si="3"/>
-        <v>4.2763636363636365E-2</v>
+        <v>0.19098181818181822</v>
       </c>
       <c r="O25">
         <f t="shared" si="4"/>
-        <v>0.11760000000000001</v>
+        <v>0.24974545454545458</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1140,26 +1254,26 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>4.9090909090909088E-2</v>
+        <v>8.1090909090909075E-2</v>
       </c>
       <c r="K26" t="s">
         <v>13</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>0.19636363636363635</v>
+        <v>0.48654545454545445</v>
       </c>
       <c r="M26">
         <f t="shared" si="2"/>
-        <v>0.1669090909090909</v>
+        <v>0.4216727272727272</v>
       </c>
       <c r="N26">
         <f t="shared" si="3"/>
-        <v>4.9090909090909088E-2</v>
+        <v>9.7309090909090887E-2</v>
       </c>
       <c r="O26">
         <f t="shared" si="4"/>
-        <v>0.108</v>
+        <v>0.19461818181818177</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1187,26 +1301,26 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>6.1090909090909085E-2</v>
+        <v>8.1090909090909088E-2</v>
       </c>
       <c r="K27" t="s">
         <v>14</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>4.8872727272727269E-2</v>
+        <v>9.7309090909090901E-2</v>
       </c>
       <c r="M27">
         <f t="shared" si="2"/>
-        <v>0.21992727272727272</v>
+        <v>0.43789090909090911</v>
       </c>
       <c r="N27">
         <f t="shared" si="3"/>
-        <v>4.8872727272727269E-2</v>
+        <v>0.12974545454545455</v>
       </c>
       <c r="O27">
         <f t="shared" si="4"/>
-        <v>0.13439999999999999</v>
+        <v>0.3081454545454545</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1234,26 +1348,26 @@
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>5.7454545454545446E-2</v>
+        <v>9.3454545454545457E-2</v>
       </c>
       <c r="K28" t="s">
         <v>15</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>0.16087272727272725</v>
+        <v>0.44858181818181819</v>
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>0.2068363636363636</v>
+        <v>0.50465454545454547</v>
       </c>
       <c r="N28">
         <f t="shared" si="3"/>
-        <v>0.1034181818181818</v>
+        <v>0.20560000000000003</v>
       </c>
       <c r="O28">
         <f t="shared" si="4"/>
-        <v>0.12639999999999998</v>
+        <v>0.29905454545454546</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1281,26 +1395,26 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>6.872727272727272E-2</v>
+        <v>8.4727272727272734E-2</v>
       </c>
       <c r="K29" t="s">
         <v>16</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>0.1512</v>
+        <v>0.28807272727272731</v>
       </c>
       <c r="M29">
         <f t="shared" si="2"/>
-        <v>0.26116363636363632</v>
+        <v>0.45752727272727278</v>
       </c>
       <c r="N29">
         <f t="shared" si="3"/>
-        <v>5.498181818181818E-2</v>
+        <v>8.4727272727272734E-2</v>
       </c>
       <c r="O29">
         <f t="shared" si="4"/>
-        <v>9.62181818181818E-2</v>
+        <v>0.22029090909090912</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1328,26 +1442,26 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>4.1090909090909088E-2</v>
+        <v>7.7090909090909085E-2</v>
       </c>
       <c r="K30" t="s">
         <v>17</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>0.15614545454545453</v>
+        <v>0.43170909090909088</v>
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>0.15614545454545453</v>
+        <v>0.43170909090909088</v>
       </c>
       <c r="N30">
         <f t="shared" si="3"/>
-        <v>2.4654545454545453E-2</v>
+        <v>6.1672727272727268E-2</v>
       </c>
       <c r="O30">
         <f t="shared" si="4"/>
-        <v>8.2181818181818175E-2</v>
+        <v>0.2621090909090909</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1362,19 +1476,19 @@
       </c>
       <c r="L32" s="4">
         <f>(L23+L24+L25+L26+L27+L28+L29+L30)</f>
-        <v>6.8510545454545451</v>
+        <v>5.3057454545454537</v>
       </c>
       <c r="M32" s="4">
         <f>(M23+M24+M25+M26+M27+M28+M29+M30)</f>
-        <v>2.6371636363636362</v>
+        <v>4.4410181818181815</v>
       </c>
       <c r="N32" s="4">
         <f>(N23+N24+N25+N26+N27+N28+N29+N30)</f>
-        <v>2.305745454545455</v>
+        <v>2.985163636363636</v>
       </c>
       <c r="O32" s="4">
         <f>(O23+O24+O25+O26+O27+O28+O29+O30)</f>
-        <v>2.7890181818181818</v>
+        <v>4.0421090909090909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized Project Selection Table
</commit_message>
<xml_diff>
--- a/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
+++ b/reports/Proposal Report/Weighted Evaluation Table for Project Selection.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA7177F-0BB1-4D04-95D0-AC90A8C6993F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Smart Connected Cat Feeding &amp; Monitoring System</t>
   </si>
@@ -88,12 +89,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Normalized Weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,24 +431,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="9.41796875" customWidth="1"/>
-    <col min="11" max="11" width="29.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -465,6 +472,9 @@
       <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
@@ -481,7 +491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -527,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -573,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -619,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -665,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -711,7 +721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -757,7 +767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -803,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -849,7 +859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>SUM(A3:A10)</f>
         <v>50</v>
@@ -859,9 +869,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="137.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:15" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -882,6 +895,9 @@
       <c r="I12" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J12" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K12" s="3" t="s">
         <v>7</v>
       </c>
@@ -898,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -922,20 +938,29 @@
         <v>9</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13">
         <f>(I13/I21)</f>
-        <v>1</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="K13" t="s">
         <v>11</v>
       </c>
       <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>8</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -958,15 +983,30 @@
       <c r="G14">
         <v>7</v>
       </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
       <c r="J14">
         <f>(I14/I21)</f>
-        <v>0</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -989,15 +1029,30 @@
       <c r="G15">
         <v>5</v>
       </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
       <c r="J15">
         <f>(I15/I21)</f>
-        <v>0</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1020,15 +1075,30 @@
       <c r="G16">
         <v>7</v>
       </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
       <c r="J16">
         <f>(I16/I21)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="K16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1051,15 +1121,30 @@
       <c r="G17">
         <v>6</v>
       </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
       <c r="J17">
         <f>(I17/I21)</f>
-        <v>0</v>
+        <v>8.9285714285714288E-2</v>
       </c>
       <c r="K17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>10</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1082,15 +1167,30 @@
       <c r="G18">
         <v>7</v>
       </c>
+      <c r="I18">
+        <v>9</v>
+      </c>
       <c r="J18">
         <f>(I18/I21)</f>
-        <v>0</v>
+        <v>0.16071428571428573</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1113,15 +1213,30 @@
       <c r="G19">
         <v>4</v>
       </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
       <c r="J19">
         <f>(I19/I21)</f>
-        <v>0</v>
+        <v>0.17857142857142858</v>
       </c>
       <c r="K19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>8</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1144,27 +1259,45 @@
       <c r="G20">
         <v>6</v>
       </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
       <c r="J20">
         <f>(I20/I21)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="K20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>7</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>(A13+A14+A15+A16+A17+A18+A19+A20)</f>
         <v>55</v>
       </c>
       <c r="I21">
         <f>(I13+I14+I15+I17+I16+I18+I19+I20)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="137.1" x14ac:dyDescent="0.55000000000000004">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>8</v>
@@ -1201,7 +1334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1226,29 +1359,29 @@
       </c>
       <c r="I23">
         <f>(B3+J3+B13+J13+B23)/5</f>
-        <v>0.25890909090909092</v>
+        <v>6.6051948051948056E-2</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
       </c>
       <c r="L23">
         <f>((D3+L3+D13+L13+D23)/5)*I23</f>
-        <v>1.7605818181818182</v>
+        <v>0.58125714285714292</v>
       </c>
       <c r="M23">
         <f>((E3+M3+E13+M13+E23)/5)*I23</f>
-        <v>1.1909818181818181</v>
+        <v>0.40952207792207795</v>
       </c>
       <c r="N23">
         <f>((F3+N3+F13+N13+F23)/5)*I23</f>
-        <v>1.6570181818181819</v>
+        <v>0.55483636363636368</v>
       </c>
       <c r="O23">
         <f>((G3+O3+G13+O13+G23)/5)*I23</f>
-        <v>1.8123636363636364</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.56804675324675324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1273,29 +1406,29 @@
       </c>
       <c r="I24">
         <f t="shared" ref="I24:I30" si="0">(B4+J4+B14+J14+B24)/5</f>
-        <v>9.0181818181818182E-2</v>
+        <v>0.11875324675324675</v>
       </c>
       <c r="K24" t="s">
         <v>12</v>
       </c>
       <c r="L24">
         <f t="shared" ref="L24:L30" si="1">((D4+L4+D14+L14+D24)/5)*I24</f>
-        <v>0.21643636363636362</v>
+        <v>0.33250909090909087</v>
       </c>
       <c r="M24">
         <f t="shared" ref="M24:M30" si="2">((E4+M4+E14+M14+E24)/5)*I24</f>
-        <v>0.45090909090909093</v>
+        <v>0.83127272727272727</v>
       </c>
       <c r="N24">
         <f t="shared" ref="N24:N30" si="3">((F4+N4+F14+N14+F24)/5)*I24</f>
-        <v>0.37876363636363636</v>
+        <v>0.61751688311688313</v>
       </c>
       <c r="O24">
         <f t="shared" ref="O24:O30" si="4">((G4+O4+G14+O14+G24)/5)*I24</f>
-        <v>0.43287272727272724</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.73627012987012985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -1320,29 +1453,29 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>9.745454545454546E-2</v>
+        <v>0.12602597402597401</v>
       </c>
       <c r="K25" t="s">
         <v>10</v>
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>0.25338181818181821</v>
+        <v>0.37807792207792201</v>
       </c>
       <c r="M25">
         <f t="shared" si="2"/>
-        <v>0.64319999999999999</v>
+        <v>1.0838233766233765</v>
       </c>
       <c r="N25">
         <f t="shared" si="3"/>
-        <v>0.27287272727272727</v>
+        <v>0.45369350649350648</v>
       </c>
       <c r="O25">
         <f t="shared" si="4"/>
-        <v>0.37032727272727273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.65533506493506488</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1367,29 +1500,29 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>0.11309090909090909</v>
+        <v>0.1380909090909091</v>
       </c>
       <c r="K26" t="s">
         <v>13</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>0.90472727272727271</v>
+        <v>1.2704363636363636</v>
       </c>
       <c r="M26">
         <f t="shared" si="2"/>
-        <v>0.81425454545454545</v>
+        <v>1.2428181818181818</v>
       </c>
       <c r="N26">
         <f t="shared" si="3"/>
-        <v>0.15832727272727271</v>
+        <v>0.22094545454545456</v>
       </c>
       <c r="O26">
         <f t="shared" si="4"/>
-        <v>0.33927272727272728</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.52474545454545451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1414,29 +1547,29 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>0.1090909090909091</v>
+        <v>0.12694805194805198</v>
       </c>
       <c r="K27" t="s">
         <v>14</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>0.24000000000000005</v>
+        <v>0.30467532467532471</v>
       </c>
       <c r="M27">
         <f t="shared" si="2"/>
-        <v>0.76363636363636367</v>
+        <v>1.1425324675324677</v>
       </c>
       <c r="N27">
         <f t="shared" si="3"/>
-        <v>0.19636363636363638</v>
+        <v>0.33006493506493517</v>
       </c>
       <c r="O27">
         <f t="shared" si="4"/>
-        <v>0.50181818181818183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.73629870129870145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -1461,29 +1594,29 @@
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>0.11345454545454545</v>
+        <v>0.14559740259740261</v>
       </c>
       <c r="K28" t="s">
         <v>15</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>0.58996363636363636</v>
+        <v>0.90270389610389623</v>
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>0.65803636363636353</v>
+        <v>1.1356597402597404</v>
       </c>
       <c r="N28">
         <f t="shared" si="3"/>
-        <v>0.29498181818181818</v>
+        <v>0.4076727272727273</v>
       </c>
       <c r="O28">
         <f t="shared" si="4"/>
-        <v>0.56727272727272726</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.90270389610389623</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1508,29 +1641,29 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>0.10072727272727273</v>
+        <v>0.13644155844155845</v>
       </c>
       <c r="K29" t="s">
         <v>16</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>0.46334545454545456</v>
+        <v>0.65491948051948057</v>
       </c>
       <c r="M29">
         <f t="shared" si="2"/>
-        <v>0.66480000000000006</v>
+        <v>1.1188207792207792</v>
       </c>
       <c r="N29">
         <f t="shared" si="3"/>
-        <v>0.12087272727272727</v>
+        <v>0.2455948051948052</v>
       </c>
       <c r="O29">
         <f t="shared" si="4"/>
-        <v>0.3223272727272728</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.54576623376623379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1555,53 +1688,53 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>0.11709090909090909</v>
+        <v>0.1420909090909091</v>
       </c>
       <c r="K30" t="s">
         <v>17</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>0.88989090909090907</v>
+        <v>1.1935636363636366</v>
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>0.88989090909090907</v>
+        <v>1.2788181818181819</v>
       </c>
       <c r="N30">
         <f t="shared" si="3"/>
-        <v>0.14050909090909092</v>
+        <v>0.19892727272727273</v>
       </c>
       <c r="O30">
         <f t="shared" si="4"/>
-        <v>0.56203636363636367</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>0.76729090909090925</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>(A23+A24+A25+A26+A27+A28+A29+A30)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K32" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L32" s="4">
         <f>(L23+L24+L25+L26+L27+L28+L29+L30)</f>
-        <v>5.3183272727272737</v>
+        <v>5.6181428571428578</v>
       </c>
       <c r="M32" s="4">
         <f>(M23+M24+M25+M26+M27+M28+M29+M30)</f>
-        <v>6.0757090909090898</v>
+        <v>8.2432675324675326</v>
       </c>
       <c r="N32" s="4">
         <f>(N23+N24+N25+N26+N27+N28+N29+N30)</f>
-        <v>3.2197090909090909</v>
+        <v>3.0292519480519484</v>
       </c>
       <c r="O32" s="4">
         <f>(O23+O24+O25+O26+O27+O28+O29+O30)</f>
-        <v>4.9082909090909093</v>
+        <v>5.4364571428571429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>